<commit_message>
Added remaining base functions
</commit_message>
<xml_diff>
--- a/velocity vs dutyCycle charracteristic.xlsx
+++ b/velocity vs dutyCycle charracteristic.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgatlaba\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harki\Documents\# School\9_Spring 2019\Adaptive_Cruise_Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658793D5-F43B-486B-A89E-1CB9940A7ED2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView minimized="1" xWindow="10524" yWindow="2604" windowWidth="23160" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>tiles</t>
   </si>
@@ -56,9 +63,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -107,18 +114,18 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,7 +188,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -441,7 +447,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -564,7 +569,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -680,7 +684,443 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5358705161854769E-2"/>
+          <c:y val="0.19486111111111112"/>
+          <c:w val="0.87753018372703417"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.16299365704286964"/>
+                  <c:y val="-6.408573928258968E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$37:$F$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25.363825363825367</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.770833333333336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.285956006768188</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.744186046511629</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65.732758620689665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>69.634703196347033</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.390243902439025</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74.754901960784309</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$37:$G$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-88F1-4665-8A93-2DEBE238B359}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="39249392"/>
+        <c:axId val="40697760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="39249392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="40697760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="40697760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="39249392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1236,6 +1676,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1253,7 +2209,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1263,6 +2225,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>29119</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>35379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>333919</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>111579</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78D23E64-93F8-4602-A6BD-604DD56ECE3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1533,11 +2531,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="70" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,20 +2739,20 @@
       <c r="G16" s="1"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F20" s="5"/>
-      <c r="G20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E21">
@@ -1830,15 +2828,119 @@
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8">
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="6">
         <f>G15/G26</f>
         <v>93.677822005995381</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>25.363825363825367</v>
+      </c>
+      <c r="G37">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>31.770833333333336</v>
+      </c>
+      <c r="G38">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>41.285956006768188</v>
+      </c>
+      <c r="G39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>56.744186046511629</v>
+      </c>
+      <c r="G40">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>65.732758620689665</v>
+      </c>
+      <c r="G41">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>69.634703196347033</v>
+      </c>
+      <c r="G42">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>74.390243902439025</v>
+      </c>
+      <c r="G43">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>74.754901960784309</v>
+      </c>
+      <c r="G44">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All stages of contoller design
</commit_message>
<xml_diff>
--- a/velocity vs dutyCycle charracteristic.xlsx
+++ b/velocity vs dutyCycle charracteristic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harki\Documents\# School\9_Spring 2019\Adaptive_Cruise_Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658793D5-F43B-486B-A89E-1CB9940A7ED2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF72291-8D43-4DC8-B620-D36B98638DF8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="10524" yWindow="2604" windowWidth="23160" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="2460" windowWidth="43200" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -699,6 +699,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Duty vs Velocity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2534,8 +2559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="70" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37:G44"/>
+    <sheetView tabSelected="1" topLeftCell="E14" zoomScale="70" workbookViewId="0">
+      <selection activeCell="T49" sqref="T49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>